<commit_message>
Finish development for Zoom and AutoAim Features
</commit_message>
<xml_diff>
--- a/validation/zoom_ratio.xlsx
+++ b/validation/zoom_ratio.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Zoom" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <numFmt numFmtId="168" formatCode="0.00000000000000000"/>
     <numFmt numFmtId="169" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="0.000000000"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -91,7 +91,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -142,7 +148,8 @@
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -176,6 +183,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1398,7 +1406,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2344,123 +2355,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C27:F36"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="27" spans="3:6">
-      <c r="C27" s="8">
+    <row r="2" spans="1:4">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="D27" s="8">
-        <f t="shared" ref="D27:D36" si="0">(((C27-1)*($E$36 - $E$27))/(MAX($C$27:$C$36) - 1))+$E$27</f>
+      <c r="B2" s="8">
+        <f t="shared" ref="B2:B11" si="0">(((A2-1)*($C$11 - $C$2))/(MAX($A$2:$A$11) - 1))+$C$2</f>
         <v>0.91</v>
       </c>
-      <c r="E27">
+      <c r="C2">
         <v>0.91</v>
       </c>
-      <c r="F27" s="9">
-        <f>E27-D27</f>
+      <c r="D2" s="9">
+        <f>C2-B2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:6">
-      <c r="C28" s="8">
+    <row r="3" spans="1:4">
+      <c r="A3" s="8">
         <v>10</v>
       </c>
-      <c r="D28" s="8">
+      <c r="B3" s="8">
         <f t="shared" si="0"/>
         <v>0.8418181818181818</v>
       </c>
     </row>
-    <row r="29" spans="3:6">
-      <c r="C29" s="8">
+    <row r="4" spans="1:4">
+      <c r="A4" s="8">
         <v>20</v>
       </c>
-      <c r="D29" s="8">
+      <c r="B4" s="8">
         <f t="shared" si="0"/>
         <v>0.76606060606060611</v>
       </c>
     </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="8">
+    <row r="5" spans="1:4">
+      <c r="A5" s="8">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="B5" s="8">
         <f t="shared" si="0"/>
         <v>0.69030303030303031</v>
       </c>
     </row>
-    <row r="31" spans="3:6">
-      <c r="C31" s="8">
+    <row r="6" spans="1:4">
+      <c r="A6" s="8">
         <v>40</v>
       </c>
-      <c r="D31" s="8">
+      <c r="B6" s="8">
         <f t="shared" si="0"/>
         <v>0.61454545454545451</v>
       </c>
     </row>
-    <row r="32" spans="3:6">
-      <c r="C32" s="8">
+    <row r="7" spans="1:4">
+      <c r="A7" s="8">
         <v>50</v>
       </c>
-      <c r="D32" s="8">
+      <c r="B7" s="8">
         <f t="shared" si="0"/>
         <v>0.53878787878787882</v>
       </c>
     </row>
-    <row r="33" spans="3:6">
-      <c r="C33" s="8">
+    <row r="8" spans="1:4">
+      <c r="A8" s="8">
         <v>60</v>
       </c>
-      <c r="D33" s="8">
+      <c r="B8" s="8">
         <f t="shared" si="0"/>
         <v>0.46303030303030307</v>
       </c>
     </row>
-    <row r="34" spans="3:6">
-      <c r="C34" s="8">
+    <row r="9" spans="1:4">
+      <c r="A9" s="8">
         <v>70</v>
       </c>
-      <c r="D34" s="8">
+      <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>0.38727272727272732</v>
       </c>
     </row>
-    <row r="35" spans="3:6">
-      <c r="C35" s="8">
+    <row r="10" spans="1:4">
+      <c r="A10" s="8">
         <v>80</v>
       </c>
-      <c r="D35" s="8">
+      <c r="B10" s="8">
         <f t="shared" si="0"/>
         <v>0.31151515151515152</v>
       </c>
     </row>
-    <row r="36" spans="3:6">
-      <c r="C36" s="8">
+    <row r="11" spans="1:4">
+      <c r="A11" s="8">
         <v>100</v>
       </c>
-      <c r="D36" s="8">
+      <c r="B11" s="8">
         <f t="shared" si="0"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="E36">
+      <c r="C11">
         <v>0.16</v>
       </c>
-      <c r="F36" s="9">
-        <f>E36-D36</f>
+      <c r="D11" s="9">
+        <f>C11-B11</f>
         <v>0</v>
       </c>
     </row>
@@ -2473,7 +2486,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2593,8 +2608,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D1401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F341" sqref="F341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2606,16 +2621,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>